<commit_message>
Check Complete Location Info Added
</commit_message>
<xml_diff>
--- a/1. Master/車両台帳　全体.xlsx
+++ b/1. Master/車両台帳　全体.xlsx
@@ -4175,6 +4175,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4183,15 +4192,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4492,7 +4492,7 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F28"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5198,13 +5198,13 @@
         <v>458</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>460</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G23" s="16" t="s">
         <v>17</v>
@@ -5233,13 +5233,13 @@
         <v>465</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>460</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="G24" s="16" t="s">
         <v>17</v>
@@ -5623,8 +5623,8 @@
       <c r="B48" s="37"/>
       <c r="C48" s="28"/>
       <c r="D48" s="28"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="72"/>
+      <c r="E48" s="75"/>
+      <c r="F48" s="75"/>
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
@@ -5634,8 +5634,8 @@
       <c r="B49" s="37"/>
       <c r="C49" s="28"/>
       <c r="D49" s="28"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="72"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
@@ -5647,8 +5647,8 @@
       <c r="D50" s="28"/>
       <c r="E50" s="28"/>
       <c r="F50" s="28"/>
-      <c r="G50" s="72"/>
-      <c r="H50" s="72"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
       <c r="I50" s="28"/>
     </row>
     <row r="51" spans="1:11">
@@ -5658,8 +5658,8 @@
       <c r="D51" s="28"/>
       <c r="E51" s="28"/>
       <c r="F51" s="28"/>
-      <c r="G51" s="72"/>
-      <c r="H51" s="72"/>
+      <c r="G51" s="75"/>
+      <c r="H51" s="75"/>
       <c r="I51" s="28"/>
     </row>
     <row r="52" spans="1:11">
@@ -5871,7 +5871,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="F24" sqref="F7:F24"/>
     </sheetView>
   </sheetViews>
@@ -6889,20 +6889,20 @@
       <c r="C50" s="42"/>
       <c r="D50" s="42"/>
       <c r="E50" s="42"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
-      <c r="I50" s="73"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="76"/>
+      <c r="H50" s="76"/>
+      <c r="I50" s="76"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="19"/>
       <c r="C51" s="42"/>
       <c r="D51" s="42"/>
       <c r="E51" s="42"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="73"/>
-      <c r="I51" s="73"/>
+      <c r="F51" s="76"/>
+      <c r="G51" s="76"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="76"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="19"/>
@@ -7331,19 +7331,19 @@
       <c r="C23" s="42"/>
       <c r="D23" s="42"/>
       <c r="E23" s="42"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
     </row>
     <row r="24" spans="3:11">
       <c r="C24" s="42"/>
       <c r="D24" s="42"/>
       <c r="E24" s="42"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
     </row>
     <row r="25" spans="3:11">
       <c r="C25" s="42"/>
@@ -7376,7 +7376,7 @@
   </sheetPr>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F17" sqref="F7:F17"/>
     </sheetView>
   </sheetViews>
@@ -7991,20 +7991,20 @@
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
       <c r="E27" s="42"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="76"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="19"/>
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
       <c r="E28" s="42"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="19"/>
@@ -8776,7 +8776,7 @@
     <row r="38" spans="1:14">
       <c r="C38" s="42"/>
       <c r="D38" s="43"/>
-      <c r="E38" s="75"/>
+      <c r="E38" s="72"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
       <c r="H38" s="38"/>
@@ -8789,8 +8789,8 @@
     </row>
     <row r="39" spans="1:14">
       <c r="C39" s="42"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="75"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="72"/>
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="38"/>
@@ -8803,8 +8803,8 @@
     </row>
     <row r="40" spans="1:14">
       <c r="C40" s="42"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="75"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="72"/>
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
       <c r="H40" s="38"/>
@@ -8818,7 +8818,7 @@
     <row r="41" spans="1:14">
       <c r="C41" s="42"/>
       <c r="D41" s="43"/>
-      <c r="E41" s="75"/>
+      <c r="E41" s="72"/>
       <c r="F41" s="38"/>
       <c r="G41" s="38"/>
       <c r="H41" s="38"/>
@@ -8832,7 +8832,7 @@
     <row r="42" spans="1:14">
       <c r="C42" s="42"/>
       <c r="D42" s="43"/>
-      <c r="E42" s="75"/>
+      <c r="E42" s="72"/>
       <c r="F42" s="38"/>
       <c r="G42" s="38"/>
       <c r="H42" s="38"/>
@@ -8846,7 +8846,7 @@
     <row r="43" spans="1:14">
       <c r="C43" s="42"/>
       <c r="D43" s="43"/>
-      <c r="E43" s="75"/>
+      <c r="E43" s="72"/>
       <c r="F43" s="38"/>
       <c r="G43" s="38"/>
       <c r="H43" s="38"/>
@@ -8859,8 +8859,8 @@
     </row>
     <row r="44" spans="1:14">
       <c r="C44" s="42"/>
-      <c r="D44" s="77"/>
-      <c r="E44" s="75"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="72"/>
       <c r="F44" s="54"/>
       <c r="G44" s="54"/>
       <c r="H44" s="54"/>
@@ -8940,7 +8940,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="F17" sqref="F7:F17"/>
     </sheetView>
   </sheetViews>
@@ -9539,20 +9539,20 @@
       <c r="C26" s="42"/>
       <c r="D26" s="42"/>
       <c r="E26" s="42"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="19"/>
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
       <c r="E27" s="42"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="76"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="19"/>
@@ -9592,7 +9592,7 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -10289,20 +10289,20 @@
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="75"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="19"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -10888,10 +10888,10 @@
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
       <c r="E21" s="42"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
       <c r="K21" s="27"/>
     </row>
     <row r="22" spans="1:11" ht="31.5" customHeight="1">
@@ -11212,10 +11212,10 @@
       <c r="C5" s="42"/>
       <c r="D5" s="42"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
       <c r="K5" s="27"/>
     </row>
     <row r="6" spans="1:11" ht="31.5" customHeight="1">

</xml_diff>